<commit_message>
revised how to read excel
</commit_message>
<xml_diff>
--- a/src/rank.xlsx
+++ b/src/rank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb2c32345b969a0e/src/challenge_in_japan/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{ABF1547C-88A3-7F42-A1D3-A8B21F9CEAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D21503B4-132B-4441-8AAB-24C686049918}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{ABF1547C-88A3-7F42-A1D3-A8B21F9CEAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EABA9E0-3307-9446-A081-E8991EFAACD9}"/>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="880" windowWidth="24940" windowHeight="22500" xr2:uid="{48730D3D-3FAC-4C45-A514-4057911DE026}"/>
+    <workbookView xWindow="4960" yWindow="3820" windowWidth="24940" windowHeight="22500" xr2:uid="{48730D3D-3FAC-4C45-A514-4057911DE026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="31">
   <si>
     <t>30sスピード</t>
     <phoneticPr fontId="1"/>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>黒田 大源</t>
+  </si>
+  <si>
+    <t>30sスピード</t>
   </si>
 </sst>
 </file>
@@ -531,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDA24DB-1514-8A42-B2FF-B8BE8869A9A7}">
-  <dimension ref="A3:D23"/>
+  <dimension ref="A4:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -545,15 +548,7 @@
     <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -566,8 +561,14 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="26">
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="26">
       <c r="A5">
         <v>1</v>
       </c>
@@ -580,8 +581,14 @@
       <c r="D5">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="26">
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="26">
       <c r="A6">
         <v>2</v>
       </c>
@@ -594,8 +601,14 @@
       <c r="D6">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="26">
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="26">
       <c r="A7">
         <v>3</v>
       </c>
@@ -608,8 +621,14 @@
       <c r="D7">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="26">
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="26">
       <c r="A8">
         <v>4</v>
       </c>
@@ -622,8 +641,14 @@
       <c r="D8">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="26">
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="26">
       <c r="A9">
         <v>5</v>
       </c>
@@ -636,8 +661,14 @@
       <c r="D9">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="26">
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="26">
       <c r="A10">
         <v>6</v>
       </c>
@@ -650,8 +681,14 @@
       <c r="D10">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="26">
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="26">
       <c r="A11">
         <v>7</v>
       </c>
@@ -664,8 +701,14 @@
       <c r="D11">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="26">
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="26">
       <c r="A12">
         <v>8</v>
       </c>
@@ -678,8 +721,14 @@
       <c r="D12">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="26">
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="26">
       <c r="A13">
         <v>9</v>
       </c>
@@ -692,8 +741,14 @@
       <c r="D13">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="26">
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="26">
       <c r="A14">
         <v>10</v>
       </c>
@@ -706,8 +761,14 @@
       <c r="D14">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="26">
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="26">
       <c r="A15">
         <v>11</v>
       </c>
@@ -720,8 +781,14 @@
       <c r="D15">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="26">
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="26">
       <c r="A16">
         <v>12</v>
       </c>
@@ -734,8 +801,14 @@
       <c r="D16">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="26">
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="26">
       <c r="A17">
         <v>13</v>
       </c>
@@ -748,8 +821,14 @@
       <c r="D17">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="26">
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="26">
       <c r="A18">
         <v>14</v>
       </c>
@@ -762,8 +841,14 @@
       <c r="D18">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="26">
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="26">
       <c r="A19">
         <v>15</v>
       </c>
@@ -776,8 +861,14 @@
       <c r="D19">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="26">
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="26">
       <c r="A20">
         <v>16</v>
       </c>
@@ -790,8 +881,14 @@
       <c r="D20">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="26">
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="26">
       <c r="A21">
         <v>17</v>
       </c>
@@ -804,8 +901,14 @@
       <c r="D21">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="26">
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="26">
       <c r="A22">
         <v>18</v>
       </c>
@@ -818,8 +921,14 @@
       <c r="D22">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="26">
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="26">
       <c r="A23">
         <v>19</v>
       </c>
@@ -831,6 +940,12 @@
       </c>
       <c r="D23">
         <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>